<commit_message>
Atualização automática de ESTANCIA_VELHA.xlsx
</commit_message>
<xml_diff>
--- a/ESTANCIA_VELHA.xlsx
+++ b/ESTANCIA_VELHA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C0F5AEE-0991-4EA9-8BE9-A3D1E4A88953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C79933D-B317-4338-B2FE-A229AA010863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,20 +22,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1163,7 +1150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1224,30 +1211,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1265,7 +1228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1299,18 +1262,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1360,7 +1318,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{D18D895E-9F43-404B-980E-1053603E1E6E}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{D170DC8F-59A6-4AA0-989D-C78EF283D244}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1390,10 +1348,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3616F2E-DE2F-4E7F-A67F-38273B09DAA5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A5A24B-038D-4DB3-B465-731B0A385C50}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1431,7 +1389,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{719D3981-02EB-4253-A849-B0F4B3EA29AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41466046-55D2-450B-BF79-FC1E36E5B155}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1494,7 +1452,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A922C2-2BC1-49FA-B18A-02CDA670A5FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2034FCA4-0E94-4086-93FE-5489928699C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1513,7 +1471,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71172975-462E-1B20-A459-AC558147DD23}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F9BC917-66E1-AA05-6409-E0C055B4A172}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1562,7 +1520,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D6ED86E-2F72-5153-7FAE-F6718FB19512}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B982030-0F93-F996-BA56-4309471DD70C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1581,7 +1539,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B8A6F1E-BD4F-8273-9CF3-883287250CD5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77FF5F70-2352-FA60-A2BC-0DC37901B87F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1612,7 +1570,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C2A99D8-ADBA-44C5-ABA1-C36C7B50CEE5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66A63DA0-6B6B-C570-083F-4FF781FD5460}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1643,7 +1601,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE96D1D9-DBB8-5512-07DC-9DEB7AF9D541}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEB95583-C50D-2A3E-8F23-5BD9FAA672F0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1686,7 +1644,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{179BAC0A-24B4-4B85-B43A-22582709A5C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E3530DB-2E59-41C3-9DBA-5B297962D744}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1724,7 +1682,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4478F72-96B7-4716-ADB6-72071B3DF447}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E47A2D22-8AD8-4A81-960A-29951E879B89}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1767,7 +1725,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB73459D-13DC-4790-8EEB-3A3F8DC30B31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02A70D21-0D0D-4D26-B1F3-8599C67C35B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2080,7 +2038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D10F8B8-D40A-45B1-A0CE-553666D139B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBBA1A5-1902-48D9-9448-491F9A282A5E}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2092,98 +2050,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="40"/>
-    <col min="6" max="6" width="2" style="40" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="40"/>
+    <col min="1" max="5" width="12.5703125" style="37"/>
+    <col min="6" max="6" width="2" style="37" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="39"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="39"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="39"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="39"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="39"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="39"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="39"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="39"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="39"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="39"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="39"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="39"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="39"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="39"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="39"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="39"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="39"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="39"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="39"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="39"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="39"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="39"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="39"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="39"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="39"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="39"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="39"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="39"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="39"/>
+      <c r="F29" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5330,19 +5288,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5376,1674 +5334,1674 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="15" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="17">
         <v>203289</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="18">
         <v>18.68</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="18">
         <v>186.8</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K2" s="19">
+      <c r="K2" s="14">
         <v>203</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="14" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="17">
         <v>433195</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="18">
         <v>34.9</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="18">
         <v>349</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K3" s="19">
+      <c r="K3" s="14">
         <v>203</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="14" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
         <v>433202</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="18">
         <v>34.9</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="18">
         <v>349</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="14">
         <v>203</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="14" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="17">
         <v>433203</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="18">
         <v>34.9</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="18">
         <v>349</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="14">
         <v>203</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="14" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="17">
         <v>433211</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="18">
         <v>34.9</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="18">
         <v>349</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="14">
         <v>203</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="14" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="17">
         <v>461193</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="18">
         <v>2105.84</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="18">
         <v>3539</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="14">
         <v>203</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="17">
         <v>461194</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="18">
         <v>2105.84</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="18">
         <v>3539</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="14">
         <v>203</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="N8" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="17">
         <v>461195</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="18">
         <v>2105.84</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="18">
         <v>3539</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="14">
         <v>203</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="N9" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="17">
         <v>461196</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="18">
         <v>2105.84</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="18">
         <v>3539</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="14">
         <v>203</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="N10" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="17">
         <v>461197</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="18">
         <v>2105.84</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="18">
         <v>3539</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="14">
         <v>203</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="17">
         <v>461198</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="18">
         <v>2105.84</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="18">
         <v>3539</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="14">
         <v>203</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="N12" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="17">
         <v>461199</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="18">
         <v>648.09</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="18">
         <v>1089</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="14">
         <v>203</v>
       </c>
-      <c r="L13" s="19" t="s">
+      <c r="L13" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M13" s="19" t="s">
+      <c r="M13" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N13" s="19" t="s">
+      <c r="N13" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="17">
         <v>461200</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="18">
         <v>648.09</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="18">
         <v>1089</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="14">
         <v>203</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M14" s="19" t="s">
+      <c r="M14" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N14" s="19" t="s">
+      <c r="N14" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="17">
         <v>461301</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="18">
         <v>648.09</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="18">
         <v>1089</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="14">
         <v>203</v>
       </c>
-      <c r="L15" s="19" t="s">
+      <c r="L15" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M15" s="19" t="s">
+      <c r="M15" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="N15" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="17">
         <v>461302</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="18">
         <v>648.09</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="18">
         <v>1089</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="14">
         <v>203</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L16" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M16" s="19" t="s">
+      <c r="M16" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N16" s="19" t="s">
+      <c r="N16" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="17">
         <v>461303</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="18">
         <v>648.09</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="18">
         <v>1089</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="14">
         <v>203</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M17" s="19" t="s">
+      <c r="M17" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N17" s="19" t="s">
+      <c r="N17" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="17">
         <v>461304</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="18">
         <v>648.09</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="18">
         <v>1089</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="14">
         <v>203</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="L18" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M18" s="19" t="s">
+      <c r="M18" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N18" s="19" t="s">
+      <c r="N18" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="17">
         <v>461305</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="18">
         <v>511.24</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="18">
         <v>859</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="14">
         <v>203</v>
       </c>
-      <c r="L19" s="19" t="s">
+      <c r="L19" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M19" s="19" t="s">
+      <c r="M19" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N19" s="19" t="s">
+      <c r="N19" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="17">
         <v>461306</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="18">
         <v>511.24</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="18">
         <v>859</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="14">
         <v>203</v>
       </c>
-      <c r="L20" s="19" t="s">
+      <c r="L20" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M20" s="19" t="s">
+      <c r="M20" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N20" s="19" t="s">
+      <c r="N20" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="17">
         <v>461307</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="18">
         <v>511.24</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="18">
         <v>859</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="14">
         <v>203</v>
       </c>
-      <c r="L21" s="19" t="s">
+      <c r="L21" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M21" s="19" t="s">
+      <c r="M21" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N21" s="19" t="s">
+      <c r="N21" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="17">
         <v>461308</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="18">
         <v>511.24</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="18">
         <v>859</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="14">
         <v>203</v>
       </c>
-      <c r="L22" s="19" t="s">
+      <c r="L22" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M22" s="19" t="s">
+      <c r="M22" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N22" s="19" t="s">
+      <c r="N22" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B23" s="20">
+      <c r="B23" s="17">
         <v>461309</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="18">
         <v>511.24</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="18">
         <v>859</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K23" s="19">
+      <c r="K23" s="14">
         <v>203</v>
       </c>
-      <c r="L23" s="19" t="s">
+      <c r="L23" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M23" s="19" t="s">
+      <c r="M23" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N23" s="19" t="s">
+      <c r="N23" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B24" s="20">
+      <c r="B24" s="17">
         <v>461310</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="18">
         <v>2017.08</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="18">
         <v>2529</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K24" s="19">
+      <c r="K24" s="14">
         <v>203</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="L24" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M24" s="19" t="s">
+      <c r="M24" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N24" s="19" t="s">
+      <c r="N24" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="17">
         <v>461311</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="18">
         <v>1422.05</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="18">
         <v>2390</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="19" t="s">
+      <c r="I25" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K25" s="19">
+      <c r="K25" s="14">
         <v>203</v>
       </c>
-      <c r="L25" s="19" t="s">
+      <c r="L25" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M25" s="19" t="s">
+      <c r="M25" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N25" s="19" t="s">
+      <c r="N25" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="17">
         <v>461312</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="18">
         <v>5777.45</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="18">
         <v>9710</v>
       </c>
-      <c r="H26" s="19" t="s">
+      <c r="H26" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I26" s="19" t="s">
+      <c r="I26" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="14">
         <v>203</v>
       </c>
-      <c r="L26" s="19" t="s">
+      <c r="L26" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M26" s="19" t="s">
+      <c r="M26" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N26" s="19" t="s">
+      <c r="N26" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="17">
         <v>461313</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="18">
         <v>433.89</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="18">
         <v>729</v>
       </c>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I27" s="19" t="s">
+      <c r="I27" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J27" s="19" t="s">
+      <c r="J27" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K27" s="19">
+      <c r="K27" s="14">
         <v>203</v>
       </c>
-      <c r="L27" s="19" t="s">
+      <c r="L27" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M27" s="19" t="s">
+      <c r="M27" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N27" s="19" t="s">
+      <c r="N27" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="17">
         <v>461314</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="18">
         <v>1289.5</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="18">
         <v>2167</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I28" s="19" t="s">
+      <c r="I28" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="J28" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K28" s="19">
+      <c r="K28" s="14">
         <v>203</v>
       </c>
-      <c r="L28" s="19" t="s">
+      <c r="L28" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M28" s="19" t="s">
+      <c r="M28" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N28" s="19" t="s">
+      <c r="N28" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="17">
         <v>461315</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="18">
         <v>310.27999999999997</v>
       </c>
-      <c r="G29" s="21">
+      <c r="G29" s="18">
         <v>521.15</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I29" s="19" t="s">
+      <c r="I29" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K29" s="14">
         <v>203</v>
       </c>
-      <c r="L29" s="19" t="s">
+      <c r="L29" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M29" s="19" t="s">
+      <c r="M29" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N29" s="19" t="s">
+      <c r="N29" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="17">
         <v>461316</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="18">
         <v>310.27999999999997</v>
       </c>
-      <c r="G30" s="21">
+      <c r="G30" s="18">
         <v>521.15</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I30" s="19" t="s">
+      <c r="I30" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J30" s="19" t="s">
+      <c r="J30" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="14">
         <v>203</v>
       </c>
-      <c r="L30" s="19" t="s">
+      <c r="L30" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M30" s="19" t="s">
+      <c r="M30" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N30" s="19" t="s">
+      <c r="N30" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="17">
         <v>461317</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="18">
         <v>310.27999999999997</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="18">
         <v>521.15</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I31" s="19" t="s">
+      <c r="I31" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J31" s="19" t="s">
+      <c r="J31" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K31" s="19">
+      <c r="K31" s="14">
         <v>203</v>
       </c>
-      <c r="L31" s="19" t="s">
+      <c r="L31" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M31" s="19" t="s">
+      <c r="M31" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N31" s="19" t="s">
+      <c r="N31" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="17">
         <v>461318</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="18">
         <v>310.27999999999997</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="18">
         <v>521.15</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J32" s="19" t="s">
+      <c r="J32" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K32" s="19">
+      <c r="K32" s="14">
         <v>203</v>
       </c>
-      <c r="L32" s="19" t="s">
+      <c r="L32" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M32" s="19" t="s">
+      <c r="M32" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N32" s="19" t="s">
+      <c r="N32" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B33" s="17">
         <v>461319</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F33" s="18">
         <v>310.27999999999997</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="18">
         <v>521.15</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I33" s="19" t="s">
+      <c r="I33" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="J33" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K33" s="19">
+      <c r="K33" s="14">
         <v>203</v>
       </c>
-      <c r="L33" s="19" t="s">
+      <c r="L33" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M33" s="19" t="s">
+      <c r="M33" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N33" s="19" t="s">
+      <c r="N33" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B34" s="20">
+      <c r="B34" s="17">
         <v>461948</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="14" t="s">
         <v>292</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="18">
         <v>2076.5500000000002</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="18">
         <v>3490</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I34" s="19" t="s">
+      <c r="I34" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J34" s="19" t="s">
+      <c r="J34" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K34" s="19">
+      <c r="K34" s="14">
         <v>203</v>
       </c>
-      <c r="L34" s="19" t="s">
+      <c r="L34" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M34" s="19" t="s">
+      <c r="M34" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N34" s="19" t="s">
+      <c r="N34" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="17">
         <v>461949</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="F35" s="21">
+      <c r="F35" s="18">
         <v>13317.29</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="18">
         <v>22382</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I35" s="19" t="s">
+      <c r="I35" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J35" s="19" t="s">
+      <c r="J35" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K35" s="19">
+      <c r="K35" s="14">
         <v>203</v>
       </c>
-      <c r="L35" s="19" t="s">
+      <c r="L35" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M35" s="19" t="s">
+      <c r="M35" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N35" s="19" t="s">
+      <c r="N35" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" s="17">
         <v>459025</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="18">
         <v>694.88</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="18">
         <v>789.6</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I36" s="19" t="s">
+      <c r="I36" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J36" s="19" t="s">
+      <c r="J36" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K36" s="19">
+      <c r="K36" s="14">
         <v>203</v>
       </c>
-      <c r="L36" s="19" t="s">
+      <c r="L36" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M36" s="19" t="s">
+      <c r="M36" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N36" s="19" t="s">
+      <c r="N36" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B37" s="20">
+      <c r="B37" s="17">
         <v>459034</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="F37" s="21">
+      <c r="F37" s="18">
         <v>980.4</v>
       </c>
-      <c r="G37" s="21">
+      <c r="G37" s="18">
         <v>1290</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I37" s="19" t="s">
+      <c r="I37" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J37" s="19" t="s">
+      <c r="J37" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K37" s="19">
+      <c r="K37" s="14">
         <v>203</v>
       </c>
-      <c r="L37" s="19" t="s">
+      <c r="L37" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M37" s="19" t="s">
+      <c r="M37" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N37" s="19" t="s">
+      <c r="N37" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" s="17">
         <v>459294</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="F38" s="21">
+      <c r="F38" s="18">
         <v>6283.05</v>
       </c>
-      <c r="G38" s="21">
+      <c r="G38" s="18">
         <v>6579.06</v>
       </c>
-      <c r="H38" s="19" t="s">
+      <c r="H38" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="I38" s="19" t="s">
+      <c r="I38" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="J38" s="19" t="s">
+      <c r="J38" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="K38" s="19">
+      <c r="K38" s="14">
         <v>203</v>
       </c>
-      <c r="L38" s="19" t="s">
+      <c r="L38" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="M38" s="19" t="s">
+      <c r="M38" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="N38" s="19" t="s">
+      <c r="N38" s="14" t="s">
         <v>282</v>
       </c>
     </row>
@@ -7061,22 +7019,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="14" t="s">
         <v>273</v>
       </c>
     </row>
@@ -7099,46 +7057,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="19" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="21" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>310</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>309</v>
       </c>
     </row>
@@ -7163,101 +7121,102 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="22" t="s">
         <v>325</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="22" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="25">
         <v>45231</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="26">
         <v>2680</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>328</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="27">
         <v>10532</v>
       </c>
-      <c r="G2" s="30">
+      <c r="G2" s="27">
         <v>1173</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="29" t="s">
         <v>331</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="29" t="s">
         <v>331</v>
       </c>
     </row>
@@ -7282,31 +7241,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>332</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="E1" s="35">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="32">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="35">
         <v>137</v>
       </c>
-      <c r="F1" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>268</v>
-      </c>
-      <c r="B2" s="38">
-        <v>137</v>
-      </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>9.0596481946832435E-3</v>
       </c>
     </row>

</xml_diff>